<commit_message>
bbc and bostonglobe (bloomberg breaks)
</commit_message>
<xml_diff>
--- a/NewsSites.xlsx
+++ b/NewsSites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattbrockman/Documents/summer_2020_projects/CoverageTrends/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCA68DE-F629-E14F-81E3-E3AB421A2D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A09CBF-DAFC-C149-B7D9-2A7A895D451E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13920" yWindow="3940" windowWidth="27540" windowHeight="17440" xr2:uid="{B255A80A-19D3-D644-8E16-C1158F5F040F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -168,6 +168,24 @@
   </si>
   <si>
     <t>axios</t>
+  </si>
+  <si>
+    <t>BBC</t>
+  </si>
+  <si>
+    <t>Boston Globe</t>
+  </si>
+  <si>
+    <t>http://www.bbc.com/</t>
+  </si>
+  <si>
+    <t>https://www.bostonglobe.com/</t>
+  </si>
+  <si>
+    <t>bbc</t>
+  </si>
+  <si>
+    <t>bostonglobe</t>
   </si>
 </sst>
 </file>
@@ -530,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5291C7-8967-304A-A643-1581167FA0DB}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,6 +745,28 @@
       </c>
       <c r="F13" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wait, did I commit this one
</commit_message>
<xml_diff>
--- a/NewsSites.xlsx
+++ b/NewsSites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattbrockman/Documents/summer_2020_projects/CoverageTrends/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A09CBF-DAFC-C149-B7D9-2A7A895D451E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5248254B-A4C9-ED4B-8A43-0DD75BAE43B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13920" yWindow="3940" windowWidth="27540" windowHeight="17440" xr2:uid="{B255A80A-19D3-D644-8E16-C1158F5F040F}"/>
   </bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
K, scraping twitter should work now
</commit_message>
<xml_diff>
--- a/NewsSites.xlsx
+++ b/NewsSites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattbrockman/Documents/summer_2020_projects/CoverageTrends/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE8DEC2-134B-D643-B312-71E60DE3BEAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7030852-BDF3-F64D-840E-05B28485837A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7020" yWindow="3400" windowWidth="20180" windowHeight="17440" xr2:uid="{B255A80A-19D3-D644-8E16-C1158F5F040F}"/>
   </bookViews>
@@ -501,7 +501,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -548,6 +548,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF657786"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -570,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -579,6 +585,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -894,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5291C7-8967-304A-A643-1581167FA0DB}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E41" sqref="A41:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1657,6 +1664,12 @@
       <c r="E40" s="2">
         <v>39308549</v>
       </c>
+    </row>
+    <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>